<commit_message>
Adding test data tables
</commit_message>
<xml_diff>
--- a/test/people.xlsx
+++ b/test/people.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cri\Cloud\SpeedToValue\Integration_APIs\TheCastle_projects\GIT_Repos\APIs4Gifts\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E4DD7DC-0E52-483C-8AFD-E9B88A86CB04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F170D3-BB58-4D01-A33C-4291213DC2FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63300" yWindow="7350" windowWidth="15390" windowHeight="9540" xr2:uid="{1364DC42-C65A-439B-829A-5D48C119C258}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>NAME</t>
   </si>
@@ -451,19 +448,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C0C440-4F50-44D6-8110-55862AE3CA16}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="20.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.9296875" customWidth="1"/>
+    <col min="3" max="3" width="20.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,127 +473,103 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>